<commit_message>
Failure Fixes + New Cases
</commit_message>
<xml_diff>
--- a/cypress/downloads/calls.xlsx
+++ b/cypress/downloads/calls.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,22 +487,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>29 camp</t>
+          <t>22 release</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Delware</t>
+          <t>Qa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>Tester</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13025724041</t>
+          <t>+923104143733</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -512,10 +512,10 @@
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45686.44011392818</v>
+        <v>45679.45525150738</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45686.44011392823</v>
+        <v>45679.45525150742</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -524,17 +524,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>29 camp</t>
+          <t>22 release</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Qa</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>Tester</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45686.44070764976</v>
+        <v>45679.45525153793</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45686.44070764979</v>
+        <v>45679.45525153796</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -561,22 +561,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>29 camp</t>
+          <t>22 release</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bt</t>
+          <t>Qa</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>bt</t>
+          <t>Tester</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+919712418524</t>
+          <t>+923104143733</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -586,12 +586,1085 @@
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45803.39244620366</v>
+        <v>45679.45525156507</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45803.3924462037</v>
+        <v>45679.45525156509</v>
       </c>
       <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45679.45525158905</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>45679.45525158906</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>45679.45525161285</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>45679.45525161287</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Delware</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13025724041</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>45679.43527089486</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>45679.43527089491</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>45679.43586353165</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45679.43586353177</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>45679.4580638584</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>45679.45806385842</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>45679.4580638987</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>45679.45806389872</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>45679.45806392523</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>45679.45806392525</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>45679.45806394615</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>45679.45806394617</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>45679.45806382405</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>45679.4580638241</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>45679.43622542399</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>45679.43622542404</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>45679.43622545911</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>45679.43622545913</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>45679.43622550167</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>45679.43622550167</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>45679.43622552588</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>45679.43622552591</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>45679.43622554796</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>45679.436225548</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>45679.43657444066</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>45679.43657444068</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>45679.43657446462</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>45679.43657446463</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>45679.4365744914</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>45679.43657449141</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>45679.43657451502</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45679.43657451505</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>45679.43657441785</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>45679.43657441788</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>45679.43716769577</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>45679.43716769579</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>45679.43716772653</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45679.43716772655</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>45679.43716775307</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>45679.43716775308</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>45679.43716778092</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>45679.43716778094</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>45679.43716766479</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>45679.43716766484</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>45679.4433783893</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>45679.44337838935</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>45679.44337842398</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>45679.443378424</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>45679.44337845234</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>45679.44337845237</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>45679.4433784759</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>45679.44337847592</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>22 release</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Qa</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>+923104143733</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>45679.44337849833</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>45679.44337849837</v>
+      </c>
+      <c r="I33" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>